<commit_message>
buffalocart error msg on resetpassword test
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_data.xlsx
+++ b/src/main/resources/Test_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\githi\IdeaProjects\buffalocart\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A461022-9B50-462F-9144-E306D40FCEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9577618-924B-4B80-A7B0-42D07DB7B3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="home" sheetId="2" r:id="rId2"/>
+    <sheet name="Recoveremail" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Login - Demo POS</t>
   </si>
@@ -34,21 +34,21 @@
     <t>HomePageTitle</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>These credentials do not match our records.</t>
   </si>
   <si>
     <t>Aju Mathew</t>
   </si>
   <si>
-    <t>valid username</t>
-  </si>
-  <si>
-    <t>valid password</t>
-  </si>
-  <si>
     <t>usergab</t>
   </si>
   <si>
@@ -56,16 +56,36 @@
   </si>
   <si>
     <t>123g</t>
+  </si>
+  <si>
+    <t>recover email id</t>
+  </si>
+  <si>
+    <t>ann76@gmail.com</t>
+  </si>
+  <si>
+    <t>reset error msg</t>
+  </si>
+  <si>
+    <t>We can't find a user with that e-mail address.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,13 +108,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,10 +409,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -400,16 +423,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>123456</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -427,14 +450,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29317059-E41C-4D32-86BD-92A4BF87CB89}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4EA08DA6-A80F-4AD0-AAEB-E901EB5D1CFA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>